<commit_message>
chore: new variables in file template_conductor_grid.xlsx
Replace variable DXINCRE with variable DXINCRE_LEFT and DXINCRE_RIGHT, used for the coarsening of the mesh to the left and to the right of the refined region respectively.

modified:   input_files/input_file_template/template_conductor_grid.xlsx
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_grid.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_grid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/input_files/input_file_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{9D3B3C21-A563-43B4-9495-3DFAB052D3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31BA4B88-10B4-41F4-B91E-D86A9C7E514F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0AD516-560B-42B3-8BF9-DA6910C10E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GRID" sheetId="1" r:id="rId1"/>
@@ -37,14 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>NELEMS</t>
   </si>
   <si>
-    <t>DXINCRE</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t xml:space="preserve">maximum spatial mesh size (if refined)                                                                                                                                      </t>
   </si>
   <si>
-    <t>size increase ratio for the spatial mesh, from initially refined zone outwards</t>
-  </si>
-  <si>
     <t xml:space="preserve">flag for mesh type: 0 = fixed and uniform; 1 = fixed refined; 3 = adapted with initial refinement; - 1 from file; in this case the z coordinates of the conductor components must be exactly the same for each conudctor component objets.                                                                     </t>
   </si>
   <si>
@@ -100,6 +94,18 @@
   </si>
   <si>
     <t xml:space="preserve"> maximum number of nodes for conductor spatial discretization</t>
+  </si>
+  <si>
+    <t>DXINCRE_LEFT</t>
+  </si>
+  <si>
+    <t>size increase ratio for the spatial mesh, used for the region to the left of the refined region.</t>
+  </si>
+  <si>
+    <t>DXINCRE_RIGHT</t>
+  </si>
+  <si>
+    <t>size increase ratio for the spatial mesh, used for the region to the right of the refined region.</t>
   </si>
 </sst>
 </file>
@@ -149,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -162,10 +168,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -176,7 +182,7 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
@@ -184,10 +190,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -565,26 +567,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:D3"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.42578125" style="9" customWidth="1"/>
     <col min="5" max="5" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="2"/>
+    <col min="6" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="str">
         <f>[1]CONDUCTOR_files!$A$1</f>
         <v>CONDUCTOR</v>
@@ -600,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -609,7 +611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
         <f>[2]TRANSIENT!A$2</f>
         <v>Variable name</v>
@@ -631,154 +633,171 @@
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="E4" s="11">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>12</v>
-      </c>
-      <c r="E6" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>13</v>
       </c>
       <c r="E7" s="10">
         <f>26</f>
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="10">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="10">
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E11" s="10">
         <v>1.2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="3">
+        <v>22</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="3">
         <v>10001</v>
       </c>
     </row>

</xml_diff>